<commit_message>
dias trabajados semana 26 feb
</commit_message>
<xml_diff>
--- a/datos/dias_trabajados.xlsx
+++ b/datos/dias_trabajados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gonza\Desktop\Repositorios\estadistica_agendamientos\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A71F0B2B-8CBC-4A58-8AD1-3215496F3AA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1816DAF-88A7-4E27-AAD3-C594CB7B2796}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -106,9 +106,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -392,12 +393,13 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.33203125" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -413,6 +415,9 @@
       <c r="D1" t="s">
         <v>8</v>
       </c>
+      <c r="E1" s="2">
+        <v>45354</v>
+      </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -427,6 +432,9 @@
       <c r="D2">
         <v>5</v>
       </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -441,6 +449,9 @@
       <c r="D3">
         <v>5</v>
       </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -453,6 +464,9 @@
         <v>3</v>
       </c>
       <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
         <v>3</v>
       </c>
     </row>
@@ -469,6 +483,9 @@
       <c r="D5">
         <v>1.2</v>
       </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -482,6 +499,9 @@
       </c>
       <c r="D6" s="1">
         <v>4</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
       </c>
       <c r="F6" s="1"/>
     </row>

</xml_diff>